<commit_message>
RESTtoApp refactoring in progress
</commit_message>
<xml_diff>
--- a/src/assets/Prometheus_Methods.xlsx
+++ b/src/assets/Prometheus_Methods.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Михаил\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Isands\Front\40_subsidy_bootstrapvue\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6109A6B1-9F46-4B80-85C9-28EF1911619E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3915" windowWidth="21600" windowHeight="11385" xr2:uid="{EA2FD33C-156D-469F-8D09-C37DF9C401C1}"/>
+    <workbookView xWindow="0" yWindow="3915" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="144">
   <si>
     <t>setConfig</t>
   </si>
@@ -442,12 +441,27 @@
   </si>
   <si>
     <t>получить данные новостной статьи</t>
+  </si>
+  <si>
+    <t>00_prometheus</t>
+  </si>
+  <si>
+    <t>проверка авторизации / получение ссылки на авторизацию ЕСИА (для неавторизованного пользователя)</t>
+  </si>
+  <si>
+    <t>changeUserCurrentProfile</t>
+  </si>
+  <si>
+    <t>getEsiaLogoutUrl</t>
+  </si>
+  <si>
+    <t>checkUserAuth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,12 +472,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -478,9 +516,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -794,18 +836,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B426B3-D21C-4492-BFEC-E01B429B5C62}">
-  <dimension ref="A1:G87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="68.5703125" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
@@ -815,35 +857,55 @@
         <v>83</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -852,7 +914,7 @@
         <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
         <v>77</v>
@@ -860,39 +922,39 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>79</v>
@@ -900,228 +962,231 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
         <v>79</v>
       </c>
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="E15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
         <v>79</v>
@@ -1132,62 +1197,62 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
         <v>79</v>
-      </c>
-      <c r="G18" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
         <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
         <v>79</v>
+      </c>
+      <c r="G19" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
         <v>79</v>
@@ -1198,42 +1263,39 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
         <v>79</v>
-      </c>
-      <c r="G21" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
         <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
         <v>79</v>
@@ -1241,62 +1303,62 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="G23" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s">
         <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F25" t="s">
         <v>79</v>
@@ -1304,39 +1366,42 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
         <v>79</v>
+      </c>
+      <c r="G26" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
         <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F27" t="s">
         <v>79</v>
@@ -1347,19 +1412,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
         <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
         <v>79</v>
@@ -1368,212 +1433,209 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" t="s">
-        <v>82</v>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" t="s">
-        <v>78</v>
+      <c r="A32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="A33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="A34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D35" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" t="s">
-        <v>54</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="F37" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="A38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="A39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
         <v>68</v>
       </c>
       <c r="E40" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F40" t="s">
         <v>79</v>
@@ -1581,19 +1643,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
         <v>68</v>
       </c>
       <c r="E41" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="F41" t="s">
         <v>79</v>
@@ -1601,19 +1663,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
         <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F42" t="s">
         <v>79</v>
@@ -1621,77 +1683,77 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
         <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F43" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>91</v>
+      <c r="A44" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B44" t="s">
         <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="D44" t="s">
         <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="F44" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" t="s">
         <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
         <v>68</v>
       </c>
       <c r="E45" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F45" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D46" t="s">
         <v>68</v>
       </c>
       <c r="E46" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F46" t="s">
         <v>79</v>
@@ -1699,19 +1761,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
         <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="F47" t="s">
         <v>79</v>
@@ -1719,19 +1781,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D48" t="s">
         <v>68</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="F48" t="s">
         <v>79</v>
@@ -1739,19 +1801,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
         <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F49" t="s">
         <v>79</v>
@@ -1759,19 +1821,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
         <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F50" t="s">
         <v>79</v>
@@ -1779,19 +1841,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D51" t="s">
         <v>68</v>
       </c>
       <c r="E51" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F51" t="s">
         <v>79</v>
@@ -1799,19 +1861,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D52" t="s">
         <v>68</v>
       </c>
       <c r="E52" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F52" t="s">
         <v>79</v>
@@ -1819,19 +1881,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D53" t="s">
         <v>68</v>
       </c>
       <c r="E53" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F53" t="s">
         <v>79</v>
@@ -1839,302 +1901,299 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D54" t="s">
         <v>68</v>
       </c>
       <c r="E54" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F54" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" t="s">
-        <v>68</v>
-      </c>
-      <c r="E55" t="s">
-        <v>114</v>
-      </c>
-      <c r="F55" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A55" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B56" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D56" t="s">
-        <v>68</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F56" t="s">
-        <v>79</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="F55" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" t="s">
         <v>116</v>
       </c>
     </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>117</v>
+      <c r="A58" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>13</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="A59" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C65" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D59" t="s">
-        <v>71</v>
-      </c>
-      <c r="E59" t="s">
-        <v>55</v>
-      </c>
-      <c r="F59" t="s">
-        <v>79</v>
-      </c>
-      <c r="G59" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" t="s">
-        <v>24</v>
-      </c>
-      <c r="C60" t="s">
-        <v>31</v>
-      </c>
-      <c r="D60" t="s">
-        <v>68</v>
-      </c>
-      <c r="E60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" t="s">
-        <v>23</v>
-      </c>
-      <c r="C61" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" t="s">
-        <v>68</v>
-      </c>
-      <c r="E61" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" t="s">
-        <v>36</v>
-      </c>
-      <c r="D62" t="s">
-        <v>68</v>
-      </c>
-      <c r="E62" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>119</v>
-      </c>
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63" t="s">
-        <v>37</v>
-      </c>
-      <c r="D63" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" t="s">
-        <v>68</v>
-      </c>
-      <c r="E64" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>121</v>
-      </c>
-      <c r="B65" t="s">
-        <v>24</v>
-      </c>
-      <c r="C65" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" t="s">
-        <v>68</v>
-      </c>
-      <c r="E65" t="s">
-        <v>54</v>
+      <c r="D65" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>122</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="A66" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D66" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" t="s">
-        <v>124</v>
+      <c r="D66" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="D67" t="s">
         <v>68</v>
       </c>
       <c r="E67" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B68" t="s">
         <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="D68" t="s">
         <v>68</v>
       </c>
       <c r="E68" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="D69" t="s">
         <v>68</v>
       </c>
       <c r="E69" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C70" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D70" t="s">
         <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="B71" t="s">
         <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D71" t="s">
         <v>68</v>
       </c>
       <c r="E71" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="B72" t="s">
         <v>24</v>
@@ -2151,262 +2210,369 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B73" t="s">
         <v>24</v>
       </c>
       <c r="C73" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D73" t="s">
         <v>68</v>
       </c>
       <c r="E73" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="B74" t="s">
         <v>24</v>
       </c>
       <c r="C74" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="D74" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E74" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C75" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D75" t="s">
         <v>69</v>
       </c>
       <c r="E75" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D76" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E76" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B77" t="s">
         <v>24</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D77" t="s">
         <v>72</v>
       </c>
       <c r="E77" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B78" t="s">
         <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D78" t="s">
         <v>72</v>
       </c>
       <c r="E78" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D79" t="s">
         <v>72</v>
       </c>
       <c r="E79" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
         <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D80" t="s">
         <v>72</v>
       </c>
       <c r="E80" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B81" t="s">
         <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D81" t="s">
         <v>72</v>
       </c>
       <c r="E81" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C82" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D82" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E82" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B83" t="s">
         <v>24</v>
       </c>
       <c r="C83" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D83" t="s">
         <v>74</v>
       </c>
       <c r="E83" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B84" t="s">
         <v>24</v>
       </c>
       <c r="C84" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D84" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E84" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
         <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D85" t="s">
         <v>75</v>
       </c>
       <c r="E85" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C86" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D86" t="s">
         <v>75</v>
       </c>
       <c r="E86" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C87" t="s">
-        <v>30</v>
-      </c>
-      <c r="D87" t="s">
-        <v>75</v>
-      </c>
-      <c r="E87" t="s">
-        <v>51</v>
+      <c r="C92" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A44:A45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
auth methods removing in App in progress
</commit_message>
<xml_diff>
--- a/src/assets/Prometheus_Methods.xlsx
+++ b/src/assets/Prometheus_Methods.xlsx
@@ -518,11 +518,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,102 +984,102 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G12" t="s">
@@ -1087,62 +1087,62 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G15" t="s">
@@ -1150,22 +1150,22 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G16" t="s">
@@ -1462,162 +1462,162 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="D33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="D34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B38" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="2" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B44" t="s">
@@ -1722,7 +1722,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+      <c r="A45" s="5"/>
       <c r="B45" t="s">
         <v>24</v>
       </c>
@@ -1920,22 +1920,22 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="3" t="s">
+      <c r="B55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="D55" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G55" t="s">
@@ -1948,19 +1948,19 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" t="s">
@@ -1971,138 +1971,138 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="3" t="s">
+      <c r="B59" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D60" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61" s="3" t="s">
+      <c r="B61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D61" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="B62" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E62" s="3" t="s">
+      <c r="D62" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63" s="3" t="s">
+      <c r="B63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="D63" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="B64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D64" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E65" s="3" t="s">
+      <c r="D65" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" s="3" t="s">
+      <c r="D66" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2452,121 +2452,121 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C89" s="5" t="s">
+      <c r="B89" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E89" s="5" t="s">
+      <c r="D89" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C90" s="5" t="s">
+      <c r="B90" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D90" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E90" s="5" t="s">
+      <c r="D90" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B91" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C91" s="5" t="s">
+      <c r="B91" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D91" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E91" s="5" t="s">
+      <c r="D91" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E92" s="2" t="s">
+      <c r="D92" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C93" s="2" t="s">
+      <c r="B93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E93" s="2" t="s">
+      <c r="D93" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C94" s="2" t="s">
+      <c r="B94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E94" s="2" t="s">
+      <c r="D94" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E95" s="2" t="s">
+      <c r="D95" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NavbarNav methods replaced in App component
</commit_message>
<xml_diff>
--- a/src/assets/Prometheus_Methods.xlsx
+++ b/src/assets/Prometheus_Methods.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="149">
   <si>
     <t>setConfig</t>
   </si>
@@ -266,9 +266,6 @@
     <t>динамический</t>
   </si>
   <si>
-    <t>лишний??</t>
-  </si>
-  <si>
     <t>должен быть изменен</t>
   </si>
   <si>
@@ -452,17 +449,35 @@
     <t>changeUserCurrentProfile</t>
   </si>
   <si>
-    <t>getEsiaLogoutUrl</t>
-  </si>
-  <si>
     <t>checkUserAuth</t>
+  </si>
+  <si>
+    <t>перенесён в App</t>
+  </si>
+  <si>
+    <t>перенесён в App, переименован в checkUserAuth</t>
+  </si>
+  <si>
+    <t>перенесён в App, переименован в getUserShortInfo</t>
+  </si>
+  <si>
+    <t>перенесён в App, переименован в getUserFullInfo</t>
+  </si>
+  <si>
+    <t>удалён</t>
+  </si>
+  <si>
+    <t>перенесён в App, переименован в signOutEsia</t>
+  </si>
+  <si>
+    <t>перенесён в App, переименован в changeUserCurrentProfile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,19 +486,21 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -493,13 +510,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,19 +533,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -839,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +875,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,150 +1001,168 @@
         <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>79</v>
+      <c r="F8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>79</v>
+      <c r="F9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>79</v>
+      <c r="F10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>79</v>
+      <c r="F11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" t="s">
-        <v>82</v>
+      <c r="F12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>79</v>
+      <c r="F13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>79</v>
+      <c r="F14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1145,31 +1184,31 @@
       <c r="F15" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G15" t="s">
-        <v>80</v>
+      <c r="G15" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1192,7 +1231,7 @@
         <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1235,7 +1274,7 @@
         <v>79</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1258,7 +1297,7 @@
         <v>79</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1321,7 +1360,7 @@
         <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1384,7 +1423,7 @@
         <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1407,7 +1446,7 @@
         <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1430,12 +1469,12 @@
         <v>79</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1462,162 +1501,162 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="D32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="2" t="s">
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="D34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="D36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="D37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="D38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="D39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1643,19 +1682,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
         <v>85</v>
       </c>
-      <c r="B41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" t="s">
         <v>86</v>
-      </c>
-      <c r="D41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E41" t="s">
-        <v>87</v>
       </c>
       <c r="F41" t="s">
         <v>79</v>
@@ -1663,19 +1702,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" t="s">
         <v>89</v>
-      </c>
-      <c r="D42" t="s">
-        <v>68</v>
-      </c>
-      <c r="E42" t="s">
-        <v>90</v>
       </c>
       <c r="F42" t="s">
         <v>79</v>
@@ -1683,26 +1722,26 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" t="s">
         <v>91</v>
       </c>
-      <c r="B43" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E43" t="s">
-        <v>92</v>
-      </c>
       <c r="F43" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B44" t="s">
@@ -1722,7 +1761,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+      <c r="A45" s="2"/>
       <c r="B45" t="s">
         <v>24</v>
       </c>
@@ -1781,19 +1820,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D48" t="s">
         <v>68</v>
       </c>
       <c r="E48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F48" t="s">
         <v>79</v>
@@ -1801,19 +1840,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
       </c>
       <c r="C49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" t="s">
         <v>97</v>
-      </c>
-      <c r="D49" t="s">
-        <v>68</v>
-      </c>
-      <c r="E49" t="s">
-        <v>98</v>
       </c>
       <c r="F49" t="s">
         <v>79</v>
@@ -1821,19 +1860,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
         <v>100</v>
       </c>
-      <c r="B50" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50" t="s">
         <v>101</v>
-      </c>
-      <c r="D50" t="s">
-        <v>68</v>
-      </c>
-      <c r="E50" t="s">
-        <v>102</v>
       </c>
       <c r="F50" t="s">
         <v>79</v>
@@ -1841,19 +1880,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
         <v>23</v>
       </c>
       <c r="C51" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51" t="s">
         <v>104</v>
-      </c>
-      <c r="D51" t="s">
-        <v>68</v>
-      </c>
-      <c r="E51" t="s">
-        <v>105</v>
       </c>
       <c r="F51" t="s">
         <v>79</v>
@@ -1861,19 +1900,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" t="s">
         <v>106</v>
       </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" t="s">
         <v>107</v>
-      </c>
-      <c r="D52" t="s">
-        <v>68</v>
-      </c>
-      <c r="E52" t="s">
-        <v>108</v>
       </c>
       <c r="F52" t="s">
         <v>79</v>
@@ -1881,19 +1920,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
       </c>
       <c r="C53" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" t="s">
         <v>109</v>
-      </c>
-      <c r="D53" t="s">
-        <v>68</v>
-      </c>
-      <c r="E53" t="s">
-        <v>110</v>
       </c>
       <c r="F53" t="s">
         <v>79</v>
@@ -1901,226 +1940,226 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" t="s">
+        <v>68</v>
+      </c>
+      <c r="E54" t="s">
         <v>113</v>
       </c>
-      <c r="B54" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F54" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" t="s">
         <v>115</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G55" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="2" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F58" t="s">
-        <v>79</v>
-      </c>
-      <c r="G58" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="D65" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="D66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D67" t="s">
         <v>68</v>
       </c>
       <c r="E67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2142,36 +2181,36 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B69" t="s">
         <v>25</v>
       </c>
       <c r="C69" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" t="s">
+        <v>68</v>
+      </c>
+      <c r="E69" t="s">
         <v>128</v>
-      </c>
-      <c r="D69" t="s">
-        <v>68</v>
-      </c>
-      <c r="E69" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
         <v>130</v>
       </c>
-      <c r="B70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
+        <v>68</v>
+      </c>
+      <c r="E70" t="s">
         <v>131</v>
-      </c>
-      <c r="D70" t="s">
-        <v>68</v>
-      </c>
-      <c r="E70" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2182,47 +2221,47 @@
         <v>24</v>
       </c>
       <c r="C71" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" t="s">
+        <v>68</v>
+      </c>
+      <c r="E71" t="s">
         <v>133</v>
-      </c>
-      <c r="D71" t="s">
-        <v>68</v>
-      </c>
-      <c r="E71" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
         <v>24</v>
       </c>
       <c r="C72" t="s">
+        <v>132</v>
+      </c>
+      <c r="D72" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72" t="s">
         <v>133</v>
-      </c>
-      <c r="D72" t="s">
-        <v>68</v>
-      </c>
-      <c r="E72" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>135</v>
+      </c>
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" t="s">
         <v>136</v>
       </c>
-      <c r="B73" t="s">
-        <v>24</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
+        <v>68</v>
+      </c>
+      <c r="E73" t="s">
         <v>137</v>
-      </c>
-      <c r="D73" t="s">
-        <v>68</v>
-      </c>
-      <c r="E73" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2448,12 +2487,12 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>24</v>
@@ -2465,12 +2504,12 @@
         <v>68</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>24</v>
@@ -2487,7 +2526,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>24</v>
@@ -2503,70 +2542,70 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E92" s="1" t="s">
+      <c r="D92" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E92" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C93" s="1" t="s">
+      <c r="A93" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E93" s="1" t="s">
+      <c r="D93" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C94" s="1" t="s">
+      <c r="B94" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E94" s="1" t="s">
+      <c r="D94" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E94" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B95" s="1" t="s">
+      <c r="A95" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E95" s="1" t="s">
+      <c r="D95" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E95" s="4" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all auth methods in App component
</commit_message>
<xml_diff>
--- a/src/assets/Prometheus_Methods.xlsx
+++ b/src/assets/Prometheus_Methods.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Isands\Front\40_subsidy_bootstrapvue\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\40_subsidy_bootstrapvue\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CBD8C0-D222-47B7-8201-9865BA4658D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3915" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="159">
   <si>
     <t>setConfig</t>
   </si>
@@ -471,12 +472,42 @@
   </si>
   <si>
     <t>перенесён в App, переименован в changeUserCurrentProfile</t>
+  </si>
+  <si>
+    <t>signInEsia</t>
+  </si>
+  <si>
+    <t>переход к форме авторизации ЕСИА</t>
+  </si>
+  <si>
+    <t>signOut</t>
+  </si>
+  <si>
+    <t>выход из системы с автоматическим определением типа ралогинивания</t>
+  </si>
+  <si>
+    <t>Авторизация</t>
+  </si>
+  <si>
+    <t>Локальная авторизация</t>
+  </si>
+  <si>
+    <t>Авторизация ЕСИА</t>
+  </si>
+  <si>
+    <t>Информация о пользователе</t>
+  </si>
+  <si>
+    <t>дубль,перенесён в App, переименован в changeUserCurrentProfile</t>
+  </si>
+  <si>
+    <t>Ролевая модель пользователя</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,7 +526,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,6 +551,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -533,12 +576,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -857,11 +903,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,210 +1051,210 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="F15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" t="s">
-        <v>81</v>
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1741,7 +1787,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B44" t="s">
@@ -1761,7 +1807,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+      <c r="A45" s="4"/>
       <c r="B45" t="s">
         <v>24</v>
       </c>
@@ -2491,121 +2537,172 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B89" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C89" s="4" t="s">
+      <c r="B90" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E89" s="4" t="s">
+      <c r="D90" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E90" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C90" s="4" t="s">
+      <c r="B99" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D90" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E90" s="4" t="s">
+      <c r="D99" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C91" s="4" t="s">
+      <c r="B100" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E91" s="4" t="s">
+      <c r="D100" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E100" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E95" s="4" t="s">
+      <c r="D102" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E102" s="3" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>